<commit_message>
update VC of BMP to value from Hafner (2020)
</commit_message>
<xml_diff>
--- a/documentation/standard_deviations_macronutrients.xlsx
+++ b/documentation/standard_deviations_macronutrients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\SimonsHardDriveSpeicher\GIT\ad_meal_prep_control\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonhellmann/Documents/GIT/ad_meal_prep_control/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4B621E-58E2-4BF2-BB03-2D09055F9C0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DECF26-2A77-274B-8A96-B420528B6FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C0D2BFA6-F474-416C-8414-9CCE1E76C4AB}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15940" xr2:uid="{C0D2BFA6-F474-416C-8414-9CCE1E76C4AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Substrate</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>cattle manure</t>
-  </si>
-  <si>
-    <t>cattle manure very uncertain</t>
   </si>
   <si>
     <t>X_ch [g/L]</t>
@@ -58,8 +55,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#,##0.00000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,9 +88,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -111,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -151,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -257,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -399,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,94 +409,88 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>23.109953294746099</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.5407885838695199</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.81720938709006496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>40.085335999999998</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.540789</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.81720899999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>21.1942560041044</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.47399297681855</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.78055438532584998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>36.613180999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.4739930000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.78055399999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>28.564458661938399</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.56011410812913898</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6.2160070986350603E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>49.423171000000004</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.560114</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.216E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>3.2058507017959101</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.77896854274625704</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.205132659585509</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>8.0146267544897896</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.94742135686564</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.51283164896377198</v>
-      </c>
+      <c r="B5" s="2">
+        <v>5.3783750000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.77896900000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.20513300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update plots of scenario 1a
nominal ideal, nominal mismatch, robust
</commit_message>
<xml_diff>
--- a/documentation/standard_deviations_macronutrients.xlsx
+++ b/documentation/standard_deviations_macronutrients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonhellmann/Documents/GIT/ad_meal_prep_control/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DECF26-2A77-274B-8A96-B420528B6FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04817C18-A0A9-F94D-86C2-E8F34BB9E148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15940" xr2:uid="{C0D2BFA6-F474-416C-8414-9CCE1E76C4AB}"/>
+    <workbookView xWindow="18800" yWindow="500" windowWidth="10000" windowHeight="15940" xr2:uid="{C0D2BFA6-F474-416C-8414-9CCE1E76C4AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>Substrate</t>
   </si>
   <si>
-    <t>maize silage</t>
-  </si>
-  <si>
     <t>grass silage</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>X_li [g/L]</t>
+  </si>
+  <si>
+    <t>corn silage</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -422,18 +422,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>40.085335999999998</v>
@@ -447,7 +447,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>36.613180999999997</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>49.423171000000004</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>5.3783750000000001</v>

</xml_diff>